<commit_message>
Fix critical bug: Use Logit-scale matching instead of probability scale
Critical Issue Fixed:
- Previously: Matching was performed on probability scale (0-1)
- Problem: Probability scale gets compressed near 0 and 1, causing distance distortion
- Now: Matching is performed on Logit scale (academic standard)

Changes:
- Convert propensity scores to Logit: logit(p) = ln(p/(1-p))
- Calculate distances on Logit scale
- Use correct caliper: 0.25 × SD of Logit scores (not probability scores)

Results Impact:
- Matching rate: 98.18% → 91.82% (more strict, but better quality)
- Post-matching avg standardized bias: 13.01% → 11.36% (improved!)
- ln_人口密度: 12.55% → 8.53% (now below 10% threshold - excellent!)

This fix ensures the analysis follows academic best practices for PSM.

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/PSM-四个变量-2009基期/PSM匹配结果汇总_四个变量.xlsx
+++ b/PSM-四个变量-2009基期/PSM匹配结果汇总_四个变量.xlsx
@@ -475,7 +475,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1:1有放回匹配</t>
+          <t>1:1有放回匹配（Logit尺度）</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.045824</t>
+          <t>0.212436</t>
         </is>
       </c>
     </row>
@@ -518,7 +518,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10">
@@ -529,7 +529,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>98.18%</t>
+          <t>91.82%</t>
         </is>
       </c>
     </row>
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12">
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>